<commit_message>
v9.5.1 - Fix coberturas especiales cotizador de retención
</commit_message>
<xml_diff>
--- a/home/static/homologacion.xlsx
+++ b/home/static/homologacion.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24334"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lazaro.gonzalez\Desktop\Widget\project\home\static\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D791DA9-A77A-4B83-812B-5B9765DE1FDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Hoja1"/>
-    <sheet r:id="rId2" sheetId="2" name="Hoja2"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Hoja1!$A$1:$D$184</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$D$184</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
+  <extLst>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="738" uniqueCount="473">
   <si>
     <t>ID_G</t>
   </si>
@@ -1434,13 +1445,15 @@
   </si>
   <si>
     <t xml:space="preserve">AMETROP/DISMIN DE AGUDEZA VISUAL (menor 2.5)B </t>
+  </si>
+  <si>
+    <t>FALSEO B_NODULOS MAMA/tiroideos/Partes blandas No</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1472,16 +1485,16 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00b0f0"/>
+        <fgColor rgb="FF00B0F0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1504,45 +1517,94 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1553,10 +1615,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1594,71 +1656,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1686,7 +1748,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1709,11 +1771,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1722,13 +1784,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1738,7 +1800,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1747,7 +1809,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1756,7 +1818,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1764,10 +1826,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1832,23 +1894,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:D184"/>
+  <dimension ref="A1:D186"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A171" workbookViewId="0">
+      <selection activeCell="B190" sqref="B190"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="7" width="5.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="53.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="61.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="61.33203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:4" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1862,7 +1926,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>138</v>
       </c>
@@ -1876,7 +1940,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>188</v>
       </c>
@@ -1890,7 +1954,7 @@
         <v>253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>197</v>
       </c>
@@ -1904,7 +1968,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>393</v>
       </c>
@@ -1918,7 +1982,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>67</v>
       </c>
@@ -1932,7 +1996,7 @@
         <v>239</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>91</v>
       </c>
@@ -1946,7 +2010,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>93</v>
       </c>
@@ -1960,7 +2024,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>94</v>
       </c>
@@ -1974,7 +2038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>96</v>
       </c>
@@ -1988,7 +2052,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>97</v>
       </c>
@@ -2002,7 +2066,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>98</v>
       </c>
@@ -2016,7 +2080,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>100</v>
       </c>
@@ -2030,7 +2094,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>101</v>
       </c>
@@ -2044,7 +2108,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>103</v>
       </c>
@@ -2058,7 +2122,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>105</v>
       </c>
@@ -2072,7 +2136,7 @@
         <v>210</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>106</v>
       </c>
@@ -2086,7 +2150,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>107</v>
       </c>
@@ -2100,7 +2164,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>108</v>
       </c>
@@ -2114,7 +2178,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>109</v>
       </c>
@@ -2128,7 +2192,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>111</v>
       </c>
@@ -2142,7 +2206,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>113</v>
       </c>
@@ -2156,7 +2220,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>114</v>
       </c>
@@ -2170,7 +2234,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>115</v>
       </c>
@@ -2184,7 +2248,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>116</v>
       </c>
@@ -2198,7 +2262,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>117</v>
       </c>
@@ -2212,7 +2276,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>118</v>
       </c>
@@ -2226,7 +2290,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>119</v>
       </c>
@@ -2240,7 +2304,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>120</v>
       </c>
@@ -2254,7 +2318,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>122</v>
       </c>
@@ -2268,7 +2332,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>124</v>
       </c>
@@ -2282,7 +2346,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>125</v>
       </c>
@@ -2296,7 +2360,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>126</v>
       </c>
@@ -2310,7 +2374,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>127</v>
       </c>
@@ -2324,7 +2388,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>128</v>
       </c>
@@ -2338,7 +2402,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>129</v>
       </c>
@@ -2352,7 +2416,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>130</v>
       </c>
@@ -2366,7 +2430,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>132</v>
       </c>
@@ -2380,7 +2444,7 @@
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>134</v>
       </c>
@@ -2394,7 +2458,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>136</v>
       </c>
@@ -2408,7 +2472,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>137</v>
       </c>
@@ -2422,7 +2486,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>140</v>
       </c>
@@ -2436,7 +2500,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>141</v>
       </c>
@@ -2450,7 +2514,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>147</v>
       </c>
@@ -2464,7 +2528,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>148</v>
       </c>
@@ -2478,7 +2542,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>149</v>
       </c>
@@ -2492,7 +2556,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>150</v>
       </c>
@@ -2506,7 +2570,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>154</v>
       </c>
@@ -2520,7 +2584,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>155</v>
       </c>
@@ -2534,7 +2598,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>158</v>
       </c>
@@ -2548,7 +2612,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>159</v>
       </c>
@@ -2562,7 +2626,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>163</v>
       </c>
@@ -2576,7 +2640,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>165</v>
       </c>
@@ -2590,7 +2654,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>175</v>
       </c>
@@ -2604,7 +2668,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>177</v>
       </c>
@@ -2618,7 +2682,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>182</v>
       </c>
@@ -2632,7 +2696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>190</v>
       </c>
@@ -2646,7 +2710,7 @@
         <v>245</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>200</v>
       </c>
@@ -2660,7 +2724,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>204</v>
       </c>
@@ -2674,7 +2738,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>226</v>
       </c>
@@ -2688,7 +2752,7 @@
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>237</v>
       </c>
@@ -2702,7 +2766,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row r="62" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>238</v>
       </c>
@@ -2716,7 +2780,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row r="63" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>241</v>
       </c>
@@ -2730,7 +2794,7 @@
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row r="64" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>243</v>
       </c>
@@ -2744,7 +2808,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row r="65" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>245</v>
       </c>
@@ -2758,7 +2822,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+    <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>247</v>
       </c>
@@ -2772,7 +2836,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+    <row r="67" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>249</v>
       </c>
@@ -2786,7 +2850,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row r="68" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>250</v>
       </c>
@@ -2800,7 +2864,7 @@
         <v>124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+    <row r="69" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>253</v>
       </c>
@@ -2814,7 +2878,7 @@
         <v>126</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row r="70" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>255</v>
       </c>
@@ -2828,7 +2892,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
+    <row r="71" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>257</v>
       </c>
@@ -2842,7 +2906,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
+    <row r="72" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>259</v>
       </c>
@@ -2856,7 +2920,7 @@
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
+    <row r="73" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>261</v>
       </c>
@@ -2870,7 +2934,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
+    <row r="74" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>264</v>
       </c>
@@ -2884,7 +2948,7 @@
         <v>276</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
+    <row r="75" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>267</v>
       </c>
@@ -2898,7 +2962,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
+    <row r="76" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>268</v>
       </c>
@@ -2912,7 +2976,7 @@
         <v>135</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
+    <row r="77" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>271</v>
       </c>
@@ -2926,7 +2990,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
+    <row r="78" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>272</v>
       </c>
@@ -2940,7 +3004,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
+    <row r="79" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>275</v>
       </c>
@@ -2954,7 +3018,7 @@
         <v>139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
+    <row r="80" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>277</v>
       </c>
@@ -2968,7 +3032,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
+    <row r="81" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>278</v>
       </c>
@@ -2982,7 +3046,7 @@
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
+    <row r="82" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>280</v>
       </c>
@@ -2996,7 +3060,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
+    <row r="83" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>283</v>
       </c>
@@ -3010,7 +3074,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
+    <row r="84" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>285</v>
       </c>
@@ -3024,7 +3088,7 @@
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
+    <row r="85" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>286</v>
       </c>
@@ -3038,7 +3102,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
+    <row r="86" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>288</v>
       </c>
@@ -3052,7 +3116,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
+    <row r="87" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>291</v>
       </c>
@@ -3066,7 +3130,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
+    <row r="88" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>292</v>
       </c>
@@ -3080,7 +3144,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
+    <row r="89" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>295</v>
       </c>
@@ -3094,7 +3158,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
+    <row r="90" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>296</v>
       </c>
@@ -3108,7 +3172,7 @@
         <v>153</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
+    <row r="91" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>299</v>
       </c>
@@ -3122,7 +3186,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
+    <row r="92" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>300</v>
       </c>
@@ -3136,7 +3200,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
+    <row r="93" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>303</v>
       </c>
@@ -3150,7 +3214,7 @@
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
+    <row r="94" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>304</v>
       </c>
@@ -3164,7 +3228,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
+    <row r="95" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>307</v>
       </c>
@@ -3178,7 +3242,7 @@
         <v>160</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
+    <row r="96" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>308</v>
       </c>
@@ -3192,7 +3256,7 @@
         <v>162</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
+    <row r="97" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>311</v>
       </c>
@@ -3206,7 +3270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
+    <row r="98" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>312</v>
       </c>
@@ -3220,7 +3284,7 @@
         <v>165</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
+    <row r="99" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>315</v>
       </c>
@@ -3234,7 +3298,7 @@
         <v>167</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
+    <row r="100" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>317</v>
       </c>
@@ -3248,7 +3312,7 @@
         <v>169</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
+    <row r="101" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>319</v>
       </c>
@@ -3262,7 +3326,7 @@
         <v>171</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
+    <row r="102" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>321</v>
       </c>
@@ -3276,7 +3340,7 @@
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
+    <row r="103" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>325</v>
       </c>
@@ -3290,7 +3354,7 @@
         <v>175</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
+    <row r="104" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>327</v>
       </c>
@@ -3304,7 +3368,7 @@
         <v>177</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
+    <row r="105" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>329</v>
       </c>
@@ -3318,7 +3382,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
+    <row r="106" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>331</v>
       </c>
@@ -3332,7 +3396,7 @@
         <v>180</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
+    <row r="107" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>332</v>
       </c>
@@ -3346,7 +3410,7 @@
         <v>182</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
+    <row r="108" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>334</v>
       </c>
@@ -3360,7 +3424,7 @@
         <v>184</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75">
+    <row r="109" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>337</v>
       </c>
@@ -3374,7 +3438,7 @@
         <v>186</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75">
+    <row r="110" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>339</v>
       </c>
@@ -3388,7 +3452,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75">
+    <row r="111" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>341</v>
       </c>
@@ -3402,7 +3466,7 @@
         <v>189</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75">
+    <row r="112" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>342</v>
       </c>
@@ -3416,7 +3480,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75">
+    <row r="113" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>345</v>
       </c>
@@ -3430,7 +3494,7 @@
         <v>192</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75">
+    <row r="114" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>347</v>
       </c>
@@ -3444,7 +3508,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75">
+    <row r="115" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>349</v>
       </c>
@@ -3458,7 +3522,7 @@
         <v>195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75">
+    <row r="116" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>352</v>
       </c>
@@ -3472,7 +3536,7 @@
         <v>197</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75">
+    <row r="117" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>355</v>
       </c>
@@ -3486,7 +3550,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75">
+    <row r="118" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>357</v>
       </c>
@@ -3500,7 +3564,7 @@
         <v>200</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75">
+    <row r="119" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>359</v>
       </c>
@@ -3514,7 +3578,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75">
+    <row r="120" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>361</v>
       </c>
@@ -3528,7 +3592,7 @@
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75">
+    <row r="121" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>363</v>
       </c>
@@ -3542,7 +3606,7 @@
         <v>205</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75">
+    <row r="122" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>365</v>
       </c>
@@ -3556,7 +3620,7 @@
         <v>207</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75">
+    <row r="123" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>367</v>
       </c>
@@ -3570,7 +3634,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75">
+    <row r="124" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>369</v>
       </c>
@@ -3584,7 +3648,7 @@
         <v>210</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75">
+    <row r="125" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>371</v>
       </c>
@@ -3598,7 +3662,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75">
+    <row r="126" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>373</v>
       </c>
@@ -3612,7 +3676,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75">
+    <row r="127" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>374</v>
       </c>
@@ -3626,7 +3690,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75">
+    <row r="128" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>376</v>
       </c>
@@ -3640,7 +3704,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75">
+    <row r="129" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>379</v>
       </c>
@@ -3654,7 +3718,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75">
+    <row r="130" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>380</v>
       </c>
@@ -3668,7 +3732,7 @@
         <v>219</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75">
+    <row r="131" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>383</v>
       </c>
@@ -3682,7 +3746,7 @@
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75">
+    <row r="132" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>384</v>
       </c>
@@ -3696,7 +3760,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75">
+    <row r="133" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>387</v>
       </c>
@@ -3710,7 +3774,7 @@
         <v>223</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75">
+    <row r="134" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>389</v>
       </c>
@@ -3724,7 +3788,7 @@
         <v>225</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75">
+    <row r="135" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>391</v>
       </c>
@@ -3738,7 +3802,7 @@
         <v>227</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75">
+    <row r="136" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>394</v>
       </c>
@@ -3752,7 +3816,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75">
+    <row r="137" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>397</v>
       </c>
@@ -3766,7 +3830,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75">
+    <row r="138" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>398</v>
       </c>
@@ -3780,7 +3844,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75">
+    <row r="139" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>401</v>
       </c>
@@ -3794,7 +3858,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75">
+    <row r="140" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>403</v>
       </c>
@@ -3808,7 +3872,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75">
+    <row r="141" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>405</v>
       </c>
@@ -3822,7 +3886,7 @@
         <v>234</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75">
+    <row r="142" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>406</v>
       </c>
@@ -3836,7 +3900,7 @@
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75">
+    <row r="143" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>409</v>
       </c>
@@ -3850,7 +3914,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75">
+    <row r="144" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>410</v>
       </c>
@@ -3864,7 +3928,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75">
+    <row r="145" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>413</v>
       </c>
@@ -3878,7 +3942,7 @@
         <v>239</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75">
+    <row r="146" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>414</v>
       </c>
@@ -3892,7 +3956,7 @@
         <v>241</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75">
+    <row r="147" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>417</v>
       </c>
@@ -3906,7 +3970,7 @@
         <v>243</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75">
+    <row r="148" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>419</v>
       </c>
@@ -3920,7 +3984,7 @@
         <v>245</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75">
+    <row r="149" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>421</v>
       </c>
@@ -3934,7 +3998,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75">
+    <row r="150" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>422</v>
       </c>
@@ -3948,7 +4012,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75">
+    <row r="151" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>425</v>
       </c>
@@ -3962,7 +4026,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75">
+    <row r="152" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>426</v>
       </c>
@@ -3976,7 +4040,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75">
+    <row r="153" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>429</v>
       </c>
@@ -3990,7 +4054,7 @@
         <v>251</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75">
+    <row r="154" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>431</v>
       </c>
@@ -4004,7 +4068,7 @@
         <v>253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75">
+    <row r="155" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>433</v>
       </c>
@@ -4018,7 +4082,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75">
+    <row r="156" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>435</v>
       </c>
@@ -4032,7 +4096,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75">
+    <row r="157" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>437</v>
       </c>
@@ -4046,7 +4110,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
+    <row r="158" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>441</v>
       </c>
@@ -4060,7 +4124,7 @@
         <v>444</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75">
+    <row r="159" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>443</v>
       </c>
@@ -4074,7 +4138,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75">
+    <row r="160" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>445</v>
       </c>
@@ -4088,7 +4152,7 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75">
+    <row r="161" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>447</v>
       </c>
@@ -4102,7 +4166,7 @@
         <v>448</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75">
+    <row r="162" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>449</v>
       </c>
@@ -4116,7 +4180,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75">
+    <row r="163" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>451</v>
       </c>
@@ -4130,7 +4194,7 @@
         <v>263</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75">
+    <row r="164" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>89</v>
       </c>
@@ -4144,7 +4208,7 @@
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75">
+    <row r="165" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>90</v>
       </c>
@@ -4158,7 +4222,7 @@
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75">
+    <row r="166" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>95</v>
       </c>
@@ -4172,7 +4236,7 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75">
+    <row r="167" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>99</v>
       </c>
@@ -4186,7 +4250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75">
+    <row r="168" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>121</v>
       </c>
@@ -4200,7 +4264,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75">
+    <row r="169" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>123</v>
       </c>
@@ -4214,7 +4278,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75">
+    <row r="170" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>133</v>
       </c>
@@ -4228,7 +4292,7 @@
         <v>195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75">
+    <row r="171" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>142</v>
       </c>
@@ -4242,7 +4306,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75">
+    <row r="172" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>143</v>
       </c>
@@ -4256,7 +4320,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75">
+    <row r="173" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>144</v>
       </c>
@@ -4270,7 +4334,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75">
+    <row r="174" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>145</v>
       </c>
@@ -4284,7 +4348,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75">
+    <row r="175" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>152</v>
       </c>
@@ -4298,7 +4362,7 @@
         <v>160</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75">
+    <row r="176" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>157</v>
       </c>
@@ -4312,7 +4376,7 @@
         <v>263</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75">
+    <row r="177" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>160</v>
       </c>
@@ -4326,7 +4390,7 @@
         <v>276</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75">
+    <row r="178" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>166</v>
       </c>
@@ -4340,7 +4404,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75">
+    <row r="179" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>168</v>
       </c>
@@ -4354,7 +4418,7 @@
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75">
+    <row r="180" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>198</v>
       </c>
@@ -4368,7 +4432,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75">
+    <row r="181" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>322</v>
       </c>
@@ -4382,7 +4446,7 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="18.75">
+    <row r="182" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
         <v>351</v>
       </c>
@@ -4396,7 +4460,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="183" customHeight="1" ht="18.75">
+    <row r="183" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
         <v>439</v>
       </c>
@@ -4410,18 +4474,46 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="18.75">
-      <c r="A184" s="3">
+    <row r="184" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A184" s="9">
         <v>453</v>
       </c>
-      <c r="B184" s="4" t="s">
+      <c r="B184" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="C184" s="3">
+      <c r="C184" s="9">
         <v>20</v>
       </c>
-      <c r="D184" s="4" t="s">
+      <c r="D184" s="10" t="s">
         <v>284</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A185" s="11">
+        <v>17</v>
+      </c>
+      <c r="B185" s="12" t="s">
+        <v>266</v>
+      </c>
+      <c r="C185" s="13">
+        <v>19</v>
+      </c>
+      <c r="D185" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A186" s="11">
+        <v>356</v>
+      </c>
+      <c r="B186" s="12" t="s">
+        <v>472</v>
+      </c>
+      <c r="C186" s="13">
+        <v>22</v>
+      </c>
+      <c r="D186" s="14" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -4430,23 +4522,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D181"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView topLeftCell="A158" workbookViewId="0">
+      <selection activeCell="D188" sqref="D188"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="7" width="5.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="53.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="8.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="8" width="59.29071428571429" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.33203125" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" hidden="1">
+    <row r="1" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4460,7 +4554,7 @@
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" hidden="1">
+    <row r="2" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3">
         <v>59</v>
       </c>
@@ -4474,7 +4568,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" hidden="1">
+    <row r="3" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>395</v>
       </c>
@@ -4488,7 +4582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" hidden="1">
+    <row r="4" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>10</v>
       </c>
@@ -4502,7 +4596,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" hidden="1">
+    <row r="5" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>13</v>
       </c>
@@ -4516,7 +4610,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" hidden="1">
+    <row r="6" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>15</v>
       </c>
@@ -4530,7 +4624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" hidden="1">
+    <row r="7" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>16</v>
       </c>
@@ -4544,7 +4638,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" hidden="1">
+    <row r="8" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>18</v>
       </c>
@@ -4558,7 +4652,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" hidden="1">
+    <row r="9" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>19</v>
       </c>
@@ -4572,7 +4666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" hidden="1">
+    <row r="10" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>20</v>
       </c>
@@ -4586,7 +4680,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" hidden="1">
+    <row r="11" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>21</v>
       </c>
@@ -4600,7 +4694,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75" hidden="1">
+    <row r="12" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>22</v>
       </c>
@@ -4614,7 +4708,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" hidden="1">
+    <row r="13" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>23</v>
       </c>
@@ -4628,7 +4722,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" hidden="1">
+    <row r="14" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>25</v>
       </c>
@@ -4642,7 +4736,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" hidden="1">
+    <row r="15" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>27</v>
       </c>
@@ -4656,7 +4750,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" hidden="1">
+    <row r="16" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>28</v>
       </c>
@@ -4670,7 +4764,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75" hidden="1">
+    <row r="17" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>29</v>
       </c>
@@ -4684,7 +4778,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75" hidden="1">
+    <row r="18" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>30</v>
       </c>
@@ -4698,7 +4792,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75" hidden="1">
+    <row r="19" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>32</v>
       </c>
@@ -4712,7 +4806,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" hidden="1">
+    <row r="20" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>34</v>
       </c>
@@ -4726,7 +4820,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75" hidden="1">
+    <row r="21" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>36</v>
       </c>
@@ -4740,7 +4834,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75" hidden="1">
+    <row r="22" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>37</v>
       </c>
@@ -4754,7 +4848,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75" hidden="1">
+    <row r="23" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>38</v>
       </c>
@@ -4768,7 +4862,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" hidden="1">
+    <row r="24" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>39</v>
       </c>
@@ -4782,7 +4876,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" hidden="1">
+    <row r="25" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>40</v>
       </c>
@@ -4796,7 +4890,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75" hidden="1">
+    <row r="26" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>41</v>
       </c>
@@ -4810,7 +4904,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75" hidden="1">
+    <row r="27" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>42</v>
       </c>
@@ -4824,7 +4918,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75" hidden="1">
+    <row r="28" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>43</v>
       </c>
@@ -4838,7 +4932,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75" hidden="1">
+    <row r="29" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>45</v>
       </c>
@@ -4852,7 +4946,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75" hidden="1">
+    <row r="30" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>46</v>
       </c>
@@ -4866,7 +4960,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75" hidden="1">
+    <row r="31" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>47</v>
       </c>
@@ -4880,7 +4974,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75" hidden="1">
+    <row r="32" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>48</v>
       </c>
@@ -4894,7 +4988,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75" hidden="1">
+    <row r="33" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>50</v>
       </c>
@@ -4908,7 +5002,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75" hidden="1">
+    <row r="34" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>51</v>
       </c>
@@ -4922,7 +5016,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75" hidden="1">
+    <row r="35" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>53</v>
       </c>
@@ -4936,7 +5030,7 @@
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75" hidden="1">
+    <row r="36" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>55</v>
       </c>
@@ -4950,7 +5044,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75" hidden="1">
+    <row r="37" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>56</v>
       </c>
@@ -4964,7 +5058,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75" hidden="1">
+    <row r="38" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>57</v>
       </c>
@@ -4978,7 +5072,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75" hidden="1">
+    <row r="39" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>58</v>
       </c>
@@ -4992,7 +5086,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75" hidden="1">
+    <row r="40" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>61</v>
       </c>
@@ -5006,7 +5100,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75" hidden="1">
+    <row r="41" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>62</v>
       </c>
@@ -5020,7 +5114,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75" hidden="1">
+    <row r="42" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>66</v>
       </c>
@@ -5034,7 +5128,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75" hidden="1">
+    <row r="43" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>68</v>
       </c>
@@ -5048,7 +5142,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75" hidden="1">
+    <row r="44" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>69</v>
       </c>
@@ -5062,7 +5156,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75" hidden="1">
+    <row r="45" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>70</v>
       </c>
@@ -5076,7 +5170,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75" hidden="1">
+    <row r="46" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>71</v>
       </c>
@@ -5090,7 +5184,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75" hidden="1">
+    <row r="47" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>75</v>
       </c>
@@ -5104,7 +5198,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75" hidden="1">
+    <row r="48" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>76</v>
       </c>
@@ -5118,7 +5212,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75" hidden="1">
+    <row r="49" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>79</v>
       </c>
@@ -5132,7 +5226,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75" hidden="1">
+    <row r="50" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>80</v>
       </c>
@@ -5146,7 +5240,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75" hidden="1">
+    <row r="51" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>83</v>
       </c>
@@ -5160,7 +5254,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75" hidden="1">
+    <row r="52" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>85</v>
       </c>
@@ -5174,7 +5268,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75" hidden="1">
+    <row r="53" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>176</v>
       </c>
@@ -5188,7 +5282,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75" hidden="1">
+    <row r="54" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>178</v>
       </c>
@@ -5202,7 +5296,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75" hidden="1">
+    <row r="55" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>194</v>
       </c>
@@ -5216,7 +5310,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75" hidden="1">
+    <row r="56" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>201</v>
       </c>
@@ -5230,7 +5324,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75" hidden="1">
+    <row r="57" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>205</v>
       </c>
@@ -5244,7 +5338,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75" hidden="1">
+    <row r="58" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>227</v>
       </c>
@@ -5258,7 +5352,7 @@
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75" hidden="1">
+    <row r="59" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>239</v>
       </c>
@@ -5272,7 +5366,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75" hidden="1">
+    <row r="60" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>240</v>
       </c>
@@ -5286,7 +5380,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75" hidden="1">
+    <row r="61" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>242</v>
       </c>
@@ -5300,7 +5394,7 @@
         <v>117</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75" hidden="1">
+    <row r="62" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>244</v>
       </c>
@@ -5314,7 +5408,7 @@
         <v>119</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75" hidden="1">
+    <row r="63" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>246</v>
       </c>
@@ -5328,7 +5422,7 @@
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75" hidden="1">
+    <row r="64" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>248</v>
       </c>
@@ -5342,7 +5436,7 @@
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75" hidden="1">
+    <row r="65" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>251</v>
       </c>
@@ -5356,7 +5450,7 @@
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75" hidden="1">
+    <row r="66" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>252</v>
       </c>
@@ -5370,7 +5464,7 @@
         <v>124</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75" hidden="1">
+    <row r="67" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>254</v>
       </c>
@@ -5384,7 +5478,7 @@
         <v>126</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75" hidden="1">
+    <row r="68" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>256</v>
       </c>
@@ -5398,7 +5492,7 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75" hidden="1">
+    <row r="69" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>258</v>
       </c>
@@ -5412,7 +5506,7 @@
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75" hidden="1">
+    <row r="70" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>260</v>
       </c>
@@ -5426,7 +5520,7 @@
         <v>130</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75" hidden="1">
+    <row r="71" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>265</v>
       </c>
@@ -5440,7 +5534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75" hidden="1">
+    <row r="72" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
         <v>266</v>
       </c>
@@ -5454,7 +5548,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75" hidden="1">
+    <row r="73" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
         <v>269</v>
       </c>
@@ -5468,7 +5562,7 @@
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75" hidden="1">
+    <row r="74" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
         <v>270</v>
       </c>
@@ -5482,7 +5576,7 @@
         <v>135</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75" hidden="1">
+    <row r="75" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
         <v>273</v>
       </c>
@@ -5496,7 +5590,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75" hidden="1">
+    <row r="76" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
         <v>274</v>
       </c>
@@ -5510,7 +5604,7 @@
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75" hidden="1">
+    <row r="77" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
         <v>276</v>
       </c>
@@ -5524,7 +5618,7 @@
         <v>139</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75" hidden="1">
+    <row r="78" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
         <v>279</v>
       </c>
@@ -5538,7 +5632,7 @@
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75" hidden="1">
+    <row r="79" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
         <v>281</v>
       </c>
@@ -5552,7 +5646,7 @@
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75" hidden="1">
+    <row r="80" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
         <v>282</v>
       </c>
@@ -5566,7 +5660,7 @@
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75" hidden="1">
+    <row r="81" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
         <v>284</v>
       </c>
@@ -5580,7 +5674,7 @@
         <v>109</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75" hidden="1">
+    <row r="82" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
         <v>287</v>
       </c>
@@ -5594,7 +5688,7 @@
         <v>146</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75" hidden="1">
+    <row r="83" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
         <v>289</v>
       </c>
@@ -5608,7 +5702,7 @@
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75" hidden="1">
+    <row r="84" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
         <v>290</v>
       </c>
@@ -5622,7 +5716,7 @@
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75" hidden="1">
+    <row r="85" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
         <v>293</v>
       </c>
@@ -5636,7 +5730,7 @@
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75" hidden="1">
+    <row r="86" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
         <v>294</v>
       </c>
@@ -5650,7 +5744,7 @@
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75" hidden="1">
+    <row r="87" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
         <v>297</v>
       </c>
@@ -5664,7 +5758,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75" hidden="1">
+    <row r="88" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
         <v>298</v>
       </c>
@@ -5678,7 +5772,7 @@
         <v>153</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75" hidden="1">
+    <row r="89" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
         <v>301</v>
       </c>
@@ -5692,7 +5786,7 @@
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75" hidden="1">
+    <row r="90" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
         <v>302</v>
       </c>
@@ -5706,7 +5800,7 @@
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75" hidden="1">
+    <row r="91" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
         <v>305</v>
       </c>
@@ -5720,7 +5814,7 @@
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75" hidden="1">
+    <row r="92" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
         <v>306</v>
       </c>
@@ -5734,7 +5828,7 @@
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75" hidden="1">
+    <row r="93" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
         <v>309</v>
       </c>
@@ -5748,7 +5842,7 @@
         <v>160</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75" hidden="1">
+    <row r="94" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
         <v>310</v>
       </c>
@@ -5762,7 +5856,7 @@
         <v>162</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75" hidden="1">
+    <row r="95" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
         <v>313</v>
       </c>
@@ -5776,7 +5870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75" hidden="1">
+    <row r="96" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
         <v>314</v>
       </c>
@@ -5790,7 +5884,7 @@
         <v>165</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75" hidden="1">
+    <row r="97" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
         <v>316</v>
       </c>
@@ -5804,7 +5898,7 @@
         <v>167</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75" hidden="1">
+    <row r="98" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
         <v>318</v>
       </c>
@@ -5818,7 +5912,7 @@
         <v>169</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75" hidden="1">
+    <row r="99" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
         <v>320</v>
       </c>
@@ -5832,7 +5926,7 @@
         <v>171</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75" hidden="1">
+    <row r="100" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
         <v>323</v>
       </c>
@@ -5846,7 +5940,7 @@
         <v>173</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75" hidden="1">
+    <row r="101" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
         <v>326</v>
       </c>
@@ -5860,7 +5954,7 @@
         <v>175</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75" hidden="1">
+    <row r="102" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
         <v>328</v>
       </c>
@@ -5874,7 +5968,7 @@
         <v>177</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75" hidden="1">
+    <row r="103" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
         <v>330</v>
       </c>
@@ -5888,7 +5982,7 @@
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75" hidden="1">
+    <row r="104" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
         <v>333</v>
       </c>
@@ -5902,7 +5996,7 @@
         <v>180</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75" hidden="1">
+    <row r="105" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
         <v>335</v>
       </c>
@@ -5916,7 +6010,7 @@
         <v>182</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75" hidden="1">
+    <row r="106" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
         <v>336</v>
       </c>
@@ -5930,7 +6024,7 @@
         <v>184</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75" hidden="1">
+    <row r="107" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
         <v>338</v>
       </c>
@@ -5944,7 +6038,7 @@
         <v>186</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75" hidden="1">
+    <row r="108" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
         <v>340</v>
       </c>
@@ -5958,7 +6052,7 @@
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="18.75" hidden="1">
+    <row r="109" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
         <v>343</v>
       </c>
@@ -5972,7 +6066,7 @@
         <v>189</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="18.75" hidden="1">
+    <row r="110" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
         <v>344</v>
       </c>
@@ -5986,7 +6080,7 @@
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="18.75" hidden="1">
+    <row r="111" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
         <v>346</v>
       </c>
@@ -6000,7 +6094,7 @@
         <v>192</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="18.75" hidden="1">
+    <row r="112" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
         <v>348</v>
       </c>
@@ -6014,7 +6108,7 @@
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="18.75" hidden="1">
+    <row r="113" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
         <v>350</v>
       </c>
@@ -6028,7 +6122,7 @@
         <v>195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="18.75" hidden="1">
+    <row r="114" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
         <v>354</v>
       </c>
@@ -6042,7 +6136,7 @@
         <v>197</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="18.75" hidden="1">
+    <row r="115" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
         <v>356</v>
       </c>
@@ -6056,7 +6150,7 @@
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="18.75" hidden="1">
+    <row r="116" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
         <v>358</v>
       </c>
@@ -6070,7 +6164,7 @@
         <v>200</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="18.75" hidden="1">
+    <row r="117" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
         <v>360</v>
       </c>
@@ -6084,7 +6178,7 @@
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="18.75" hidden="1">
+    <row r="118" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
         <v>362</v>
       </c>
@@ -6098,7 +6192,7 @@
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="18.75" hidden="1">
+    <row r="119" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
         <v>364</v>
       </c>
@@ -6112,7 +6206,7 @@
         <v>205</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="18.75" hidden="1">
+    <row r="120" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
         <v>366</v>
       </c>
@@ -6126,7 +6220,7 @@
         <v>207</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="18.75" hidden="1">
+    <row r="121" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
         <v>368</v>
       </c>
@@ -6140,7 +6234,7 @@
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="18.75" hidden="1">
+    <row r="122" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
         <v>370</v>
       </c>
@@ -6154,7 +6248,7 @@
         <v>210</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="18.75" hidden="1">
+    <row r="123" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
         <v>372</v>
       </c>
@@ -6168,7 +6262,7 @@
         <v>212</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="18.75" hidden="1">
+    <row r="124" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
         <v>375</v>
       </c>
@@ -6182,7 +6276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="18.75" hidden="1">
+    <row r="125" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
         <v>377</v>
       </c>
@@ -6196,7 +6290,7 @@
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="18.75" hidden="1">
+    <row r="126" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
         <v>378</v>
       </c>
@@ -6210,7 +6304,7 @@
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="18.75" hidden="1">
+    <row r="127" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
         <v>381</v>
       </c>
@@ -6224,7 +6318,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="18.75" hidden="1">
+    <row r="128" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
         <v>382</v>
       </c>
@@ -6238,7 +6332,7 @@
         <v>219</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="18.75" hidden="1">
+    <row r="129" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
         <v>385</v>
       </c>
@@ -6252,7 +6346,7 @@
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="18.75" hidden="1">
+    <row r="130" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
         <v>386</v>
       </c>
@@ -6266,7 +6360,7 @@
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18.75" hidden="1">
+    <row r="131" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
         <v>388</v>
       </c>
@@ -6280,7 +6374,7 @@
         <v>223</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="18.75" hidden="1">
+    <row r="132" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
         <v>390</v>
       </c>
@@ -6294,7 +6388,7 @@
         <v>225</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="18.75" hidden="1">
+    <row r="133" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
         <v>392</v>
       </c>
@@ -6308,7 +6402,7 @@
         <v>227</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="18.75" hidden="1">
+    <row r="134" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
         <v>396</v>
       </c>
@@ -6322,7 +6416,7 @@
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="135" customHeight="1" ht="18.75" hidden="1">
+    <row r="135" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
         <v>399</v>
       </c>
@@ -6336,7 +6430,7 @@
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="136" customHeight="1" ht="18.75" hidden="1">
+    <row r="136" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
         <v>400</v>
       </c>
@@ -6350,7 +6444,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="137" customHeight="1" ht="18.75" hidden="1">
+    <row r="137" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
         <v>402</v>
       </c>
@@ -6364,7 +6458,7 @@
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="138" customHeight="1" ht="18.75" hidden="1">
+    <row r="138" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
         <v>404</v>
       </c>
@@ -6378,7 +6472,7 @@
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="18.75" hidden="1">
+    <row r="139" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
         <v>407</v>
       </c>
@@ -6392,7 +6486,7 @@
         <v>234</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="140" customHeight="1" ht="18.75" hidden="1">
+    <row r="140" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
         <v>408</v>
       </c>
@@ -6406,7 +6500,7 @@
         <v>111</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="18.75" hidden="1">
+    <row r="141" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
         <v>411</v>
       </c>
@@ -6420,7 +6514,7 @@
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="18.75" hidden="1">
+    <row r="142" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
         <v>412</v>
       </c>
@@ -6434,7 +6528,7 @@
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="18.75" hidden="1">
+    <row r="143" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
         <v>415</v>
       </c>
@@ -6448,7 +6542,7 @@
         <v>239</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="144" customHeight="1" ht="18.75" hidden="1">
+    <row r="144" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
         <v>416</v>
       </c>
@@ -6462,7 +6556,7 @@
         <v>241</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="145" customHeight="1" ht="18.75" hidden="1">
+    <row r="145" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
         <v>418</v>
       </c>
@@ -6476,7 +6570,7 @@
         <v>243</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="18.75" hidden="1">
+    <row r="146" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
         <v>420</v>
       </c>
@@ -6490,7 +6584,7 @@
         <v>245</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="18.75" hidden="1">
+    <row r="147" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
         <v>423</v>
       </c>
@@ -6504,7 +6598,7 @@
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="18.75" hidden="1">
+    <row r="148" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
         <v>424</v>
       </c>
@@ -6518,7 +6612,7 @@
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="18.75" hidden="1">
+    <row r="149" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
         <v>427</v>
       </c>
@@ -6532,7 +6626,7 @@
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="150" customHeight="1" ht="18.75" hidden="1">
+    <row r="150" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
         <v>428</v>
       </c>
@@ -6546,7 +6640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="151" customHeight="1" ht="18.75" hidden="1">
+    <row r="151" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
         <v>430</v>
       </c>
@@ -6560,7 +6654,7 @@
         <v>251</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="152" customHeight="1" ht="18.75" hidden="1">
+    <row r="152" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
         <v>432</v>
       </c>
@@ -6574,7 +6668,7 @@
         <v>253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="18.75" hidden="1">
+    <row r="153" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
         <v>434</v>
       </c>
@@ -6588,7 +6682,7 @@
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="18.75" hidden="1">
+    <row r="154" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
         <v>436</v>
       </c>
@@ -6602,7 +6696,7 @@
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="155" customHeight="1" ht="18.75" hidden="1">
+    <row r="155" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
         <v>438</v>
       </c>
@@ -6616,7 +6710,7 @@
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="156" customHeight="1" ht="18.75" hidden="1">
+    <row r="156" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
         <v>444</v>
       </c>
@@ -6630,7 +6724,7 @@
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="18.75" hidden="1">
+    <row r="157" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
         <v>446</v>
       </c>
@@ -6644,7 +6738,7 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="18.75">
+    <row r="158" spans="1:4" ht="144.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
         <v>448</v>
       </c>
@@ -6658,7 +6752,7 @@
         <v>171</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="18.75" hidden="1">
+    <row r="159" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
         <v>450</v>
       </c>
@@ -6672,7 +6766,7 @@
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="18.75" hidden="1">
+    <row r="160" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
         <v>452</v>
       </c>
@@ -6686,7 +6780,7 @@
         <v>263</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="18.75" hidden="1">
+    <row r="161" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
         <v>11</v>
       </c>
@@ -6700,7 +6794,7 @@
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="162" customHeight="1" ht="18.75" hidden="1">
+    <row r="162" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
         <v>12</v>
       </c>
@@ -6714,7 +6808,7 @@
         <v>203</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="163" customHeight="1" ht="18.75" hidden="1">
+    <row r="163" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
         <v>17</v>
       </c>
@@ -6728,7 +6822,7 @@
         <v>259</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="164" customHeight="1" ht="18.75" hidden="1">
+    <row r="164" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
         <v>44</v>
       </c>
@@ -6742,7 +6836,7 @@
         <v>115</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="165" customHeight="1" ht="18.75" hidden="1">
+    <row r="165" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
         <v>49</v>
       </c>
@@ -6756,7 +6850,7 @@
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="166" customHeight="1" ht="18.75" hidden="1">
+    <row r="166" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
         <v>54</v>
       </c>
@@ -6770,7 +6864,7 @@
         <v>195</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="18.75" hidden="1">
+    <row r="167" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
         <v>63</v>
       </c>
@@ -6784,7 +6878,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="18.75" hidden="1">
+    <row r="168" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
         <v>64</v>
       </c>
@@ -6798,7 +6892,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="18.75" hidden="1">
+    <row r="169" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
         <v>65</v>
       </c>
@@ -6812,7 +6906,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="18.75" hidden="1">
+    <row r="170" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
         <v>73</v>
       </c>
@@ -6826,7 +6920,7 @@
         <v>160</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="18.75" hidden="1">
+    <row r="171" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
         <v>78</v>
       </c>
@@ -6840,7 +6934,7 @@
         <v>263</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="18.75" hidden="1">
+    <row r="172" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
         <v>81</v>
       </c>
@@ -6854,7 +6948,7 @@
         <v>276</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="18.75" hidden="1">
+    <row r="173" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
         <v>86</v>
       </c>
@@ -6868,7 +6962,7 @@
         <v>113</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="18.75" hidden="1">
+    <row r="174" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
         <v>88</v>
       </c>
@@ -6882,7 +6976,7 @@
         <v>142</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="18.75" hidden="1">
+    <row r="175" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
         <v>146</v>
       </c>
@@ -6896,7 +6990,7 @@
         <v>239</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="18.75" hidden="1">
+    <row r="176" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
         <v>189</v>
       </c>
@@ -6910,7 +7004,7 @@
         <v>253</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="18.75" hidden="1">
+    <row r="177" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
         <v>191</v>
       </c>
@@ -6924,7 +7018,7 @@
         <v>245</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="18.75" hidden="1">
+    <row r="178" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
         <v>199</v>
       </c>
@@ -6938,7 +7032,7 @@
         <v>217</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="18.75" hidden="1">
+    <row r="179" spans="1:4" ht="18.75" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
         <v>324</v>
       </c>
@@ -6952,7 +7046,7 @@
         <v>284</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="18.75" hidden="1">
+    <row r="180" spans="1:4" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
         <v>353</v>
       </c>
@@ -6966,7 +7060,7 @@
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="18.75" hidden="1">
+    <row r="181" spans="1:4" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
         <v>440</v>
       </c>

</xml_diff>